<commit_message>
update project schedule - mandays
</commit_message>
<xml_diff>
--- a/Documentation/[FHF]_Report2_Project Schedule.xlsx
+++ b/Documentation/[FHF]_Report2_Project Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Semester9\SEP490\fu-house-finder\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28890D0A-B83E-4095-8FDE-E0C5A6A05CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9902C83-89DB-4D44-B27F-A7785DA1D042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="123">
   <si>
     <t>Name</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Initiation (Stage 1)</t>
   </si>
   <si>
-    <t>19 days</t>
-  </si>
-  <si>
     <t>Week 1-2-3</t>
   </si>
   <si>
@@ -88,15 +85,9 @@
     <t>Prepare Report 1</t>
   </si>
   <si>
-    <t>14 days</t>
-  </si>
-  <si>
     <t>Design Database</t>
   </si>
   <si>
-    <t>11 days</t>
-  </si>
-  <si>
     <t>8SS</t>
   </si>
   <si>
@@ -109,9 +100,6 @@
     <t>Draw Use Case Diagram</t>
   </si>
   <si>
-    <t>23days</t>
-  </si>
-  <si>
     <t>Draw Screen Mockup</t>
   </si>
   <si>
@@ -136,9 +124,6 @@
     <t>Planning &amp; Requirement (Stage 2)</t>
   </si>
   <si>
-    <t>7 days</t>
-  </si>
-  <si>
     <t>Project Planning</t>
   </si>
   <si>
@@ -148,9 +133,6 @@
     <t>Prepare Project Plan</t>
   </si>
   <si>
-    <t>4 days</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
@@ -169,18 +151,12 @@
     <t>Requirement Analyzing</t>
   </si>
   <si>
-    <t>3 days</t>
-  </si>
-  <si>
     <t>Week 4-5</t>
   </si>
   <si>
     <t>Write SRS</t>
   </si>
   <si>
-    <t>15+ 5days</t>
-  </si>
-  <si>
     <t>Update Project Plan</t>
   </si>
   <si>
@@ -223,9 +199,6 @@
     <t>Code Iteration 1</t>
   </si>
   <si>
-    <t>13 days</t>
-  </si>
-  <si>
     <t>29</t>
   </si>
   <si>
@@ -250,18 +223,12 @@
     <t>Code Iteration 2</t>
   </si>
   <si>
-    <t>43 days</t>
-  </si>
-  <si>
     <t>35</t>
   </si>
   <si>
     <t>Create Test Cases (Iteration 2)</t>
   </si>
   <si>
-    <t>32 days</t>
-  </si>
-  <si>
     <t>37</t>
   </si>
   <si>
@@ -307,9 +274,6 @@
     <t>Transition (Stage 6)</t>
   </si>
   <si>
-    <t>12 days</t>
-  </si>
-  <si>
     <t>Week 14-15</t>
   </si>
   <si>
@@ -361,9 +325,6 @@
     <t>19/12/2022</t>
   </si>
   <si>
-    <t>106 days</t>
-  </si>
-  <si>
     <t>Deliver Report 4</t>
   </si>
   <si>
@@ -383,6 +344,51 @@
   </si>
   <si>
     <t>Deliver Report 5 (Test Report)</t>
+  </si>
+  <si>
+    <t>337 days</t>
+  </si>
+  <si>
+    <t>9 days</t>
+  </si>
+  <si>
+    <t>20 days</t>
+  </si>
+  <si>
+    <t>25 days</t>
+  </si>
+  <si>
+    <t>30 days</t>
+  </si>
+  <si>
+    <t>58 days</t>
+  </si>
+  <si>
+    <t>26 days</t>
+  </si>
+  <si>
+    <t>33 days</t>
+  </si>
+  <si>
+    <t>31 days</t>
+  </si>
+  <si>
+    <t>60 days</t>
+  </si>
+  <si>
+    <t>15 days</t>
+  </si>
+  <si>
+    <t>6 days</t>
+  </si>
+  <si>
+    <t>156 days</t>
+  </si>
+  <si>
+    <t>78 days</t>
+  </si>
+  <si>
+    <t>62 days</t>
   </si>
 </sst>
 </file>
@@ -392,7 +398,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,6 +425,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -482,10 +494,10 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,7 +823,8 @@
     <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -821,25 +834,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -848,16 +861,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D2" s="8">
         <v>44810.333333333336</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="7"/>
@@ -871,7 +884,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D3" s="11">
         <v>44810.333333333336</v>
@@ -891,7 +904,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>10</v>
+        <v>113</v>
       </c>
       <c r="D4" s="8">
         <v>44810.333333333336</v>
@@ -902,7 +915,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -910,10 +923,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="D5" s="11">
         <v>44810.333333333336</v>
@@ -922,7 +935,7 @@
         <v>44810.333333333336</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -932,10 +945,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="D6" s="11">
         <v>44811.333333333336</v>
@@ -944,7 +957,7 @@
         <v>44811.333333333336</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -954,10 +967,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="D7" s="11">
         <v>44812</v>
@@ -966,7 +979,7 @@
         <v>44814</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -976,10 +989,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
       <c r="D8" s="11">
         <v>44814.333333333336</v>
@@ -997,11 +1010,11 @@
       <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>23</v>
+      <c r="B9" s="15" t="s">
+        <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="D9" s="11">
         <v>44811</v>
@@ -1010,7 +1023,7 @@
         <v>44822</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -1020,10 +1033,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>24</v>
+        <v>110</v>
       </c>
       <c r="D10" s="11">
         <v>44811.333333333336</v>
@@ -1041,11 +1054,11 @@
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>27</v>
+      <c r="B11" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="11">
         <v>44822.333333333336</v>
@@ -1063,11 +1076,11 @@
       <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>28</v>
+      <c r="B12" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D12" s="11">
         <v>44824.333333333336</v>
@@ -1085,11 +1098,11 @@
       <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>30</v>
+      <c r="B13" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D13" s="11">
         <v>44827.333333333336</v>
@@ -1098,7 +1111,7 @@
         <v>44828.333333333336</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -1107,11 +1120,11 @@
       <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>33</v>
+      <c r="B14" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D14" s="11">
         <v>44828</v>
@@ -1120,7 +1133,7 @@
         <v>44829</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -1130,10 +1143,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D15" s="11">
         <v>44828.333333333336</v>
@@ -1142,7 +1155,7 @@
         <v>44829</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -1152,16 +1165,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>38</v>
+        <v>117</v>
       </c>
       <c r="D16" s="7">
         <v>44830</v>
       </c>
       <c r="E16" s="7">
-        <v>44836</v>
+        <v>44844</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="7"/>
@@ -1172,13 +1185,17 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+        <v>114</v>
+      </c>
+      <c r="D17" s="7">
+        <v>44830</v>
+      </c>
+      <c r="E17" s="7">
+        <v>44843</v>
+      </c>
       <c r="F17" s="5"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -1188,19 +1205,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
       <c r="D18" s="4">
         <v>44830</v>
       </c>
       <c r="E18" s="4">
-        <v>44834</v>
+        <v>44843</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -1210,19 +1227,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D19" s="4">
-        <v>44834</v>
+        <v>44843</v>
       </c>
       <c r="E19" s="4">
-        <v>44835</v>
+        <v>44844</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -1232,10 +1249,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D20" s="7">
         <v>44828</v>
@@ -1252,10 +1269,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D21" s="4">
         <v>44828</v>
@@ -1272,10 +1289,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>49</v>
+        <v>115</v>
       </c>
       <c r="D22" s="7">
         <v>44834</v>
@@ -1286,7 +1303,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1294,10 +1311,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>49</v>
+        <v>112</v>
       </c>
       <c r="D23" s="4">
         <v>44834</v>
@@ -1305,9 +1322,7 @@
       <c r="E23" s="4">
         <v>44836</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="F23" s="5"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
@@ -1316,10 +1331,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D24" s="4">
         <v>44836</v>
@@ -1328,7 +1343,7 @@
         <v>44836</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -1338,10 +1353,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D25" s="4">
         <v>44836</v>
@@ -1350,7 +1365,7 @@
         <v>44836</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -1360,10 +1375,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
       <c r="D26" s="7">
         <v>44834</v>
@@ -1374,7 +1389,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1382,10 +1397,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="D27" s="4">
         <v>44834</v>
@@ -1394,7 +1409,7 @@
         <v>44844</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -1404,10 +1419,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D28" s="4">
         <v>44844</v>
@@ -1416,7 +1431,7 @@
         <v>44849</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -1426,10 +1441,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D29" s="4">
         <v>44849</v>
@@ -1438,7 +1453,7 @@
         <v>44850</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
@@ -1448,10 +1463,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="D30" s="7">
         <v>44851</v>
@@ -1462,7 +1477,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1470,10 +1485,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="D31" s="7">
         <v>44851</v>
@@ -1490,10 +1505,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D32" s="4">
         <v>44851</v>
@@ -1502,7 +1517,7 @@
         <v>44855</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -1512,10 +1527,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D33" s="4">
         <v>44856</v>
@@ -1524,7 +1539,7 @@
         <v>44859</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
@@ -1534,10 +1549,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>38</v>
+        <v>122</v>
       </c>
       <c r="D34" s="4">
         <v>44856</v>
@@ -1546,7 +1561,7 @@
         <v>44863</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
@@ -1556,10 +1571,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D35" s="4">
         <v>44864</v>
@@ -1568,7 +1583,7 @@
         <v>44864</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
@@ -1578,10 +1593,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="D36" s="7">
         <v>44865</v>
@@ -1598,10 +1613,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D37" s="4">
         <v>44865</v>
@@ -1610,7 +1625,7 @@
         <v>44869</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
@@ -1620,10 +1635,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="D38" s="4">
         <v>44874</v>
@@ -1632,7 +1647,7 @@
         <v>44877</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
@@ -1642,10 +1657,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="D39" s="4">
         <v>44874</v>
@@ -1654,7 +1669,7 @@
         <v>44906</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
@@ -1664,10 +1679,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D40" s="4">
         <v>44906</v>
@@ -1676,7 +1691,7 @@
         <v>44906</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
@@ -1686,10 +1701,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D41" s="4">
         <v>44907</v>
@@ -1698,7 +1713,7 @@
         <v>44907</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
@@ -1708,10 +1723,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D42" s="7">
         <v>44907</v>
@@ -1722,7 +1737,7 @@
       <c r="F42" s="10"/>
       <c r="G42" s="7"/>
       <c r="H42" s="7" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1730,10 +1745,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D43" s="4">
         <v>44907</v>
@@ -1742,7 +1757,7 @@
         <v>44912</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
@@ -1752,10 +1767,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D44" s="4">
         <v>44907</v>
@@ -1764,7 +1779,7 @@
         <v>44912</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
@@ -1774,10 +1789,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D45" s="4">
         <v>44907</v>
@@ -1786,7 +1801,7 @@
         <v>44912</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
@@ -1796,10 +1811,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D46" s="4">
         <v>44912</v>
@@ -1808,7 +1823,7 @@
         <v>44912</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
@@ -1818,21 +1833,21 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="D47" s="7">
         <v>44912</v>
       </c>
       <c r="E47" s="7">
-        <v>44913</v>
+        <v>44914</v>
       </c>
       <c r="F47" s="10"/>
       <c r="G47" s="7"/>
       <c r="H47" s="7" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1840,13 +1855,17 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
+        <v>119</v>
+      </c>
+      <c r="D48" s="7">
+        <v>44912</v>
+      </c>
+      <c r="E48" s="7">
+        <v>44913</v>
+      </c>
       <c r="F48" s="5"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
@@ -1856,10 +1875,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D49" s="4">
         <v>44912</v>
@@ -1868,7 +1887,7 @@
         <v>44913</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
@@ -1878,10 +1897,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D50" s="4">
         <v>44912</v>
@@ -1890,7 +1909,7 @@
         <v>44913</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
@@ -1900,10 +1919,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D51" s="4">
         <v>44912</v>
@@ -1912,7 +1931,7 @@
         <v>44913</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
@@ -1922,21 +1941,21 @@
         <v>51</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D52" s="4">
-        <v>44907</v>
-      </c>
-      <c r="E52" s="4">
-        <v>44914</v>
+        <v>109</v>
+      </c>
+      <c r="D52" s="7">
+        <v>44912</v>
+      </c>
+      <c r="E52" s="7">
+        <v>44913</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="4"/>
       <c r="H52" s="7" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -1944,10 +1963,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D53" s="4">
         <v>44907</v>
@@ -1956,7 +1975,7 @@
         <v>44912</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
@@ -1966,7 +1985,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>8</v>
@@ -1978,7 +1997,7 @@
         <v>44912</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
@@ -1988,10 +2007,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D55" s="4">
         <v>44911</v>
@@ -2000,7 +2019,7 @@
         <v>44913</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
@@ -2010,10 +2029,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D56" s="4">
         <v>44913</v>
@@ -2022,7 +2041,7 @@
         <v>44914</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
@@ -2032,10 +2051,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D57" s="4">
         <v>44913</v>
@@ -2044,7 +2063,7 @@
         <v>44914</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>

</xml_diff>